<commit_message>
Update EPCI import to handle 2023 files
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/intercommunalites.xlsx
+++ b/spec/fixtures/files/intercommunalites.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ink/dev/fiscahub/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3179AC-1192-2347-BD00-8B77EAF7FA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604FFADB-D802-0547-BFFE-AD4521202285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20140" yWindow="500" windowWidth="27640" windowHeight="26500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20120" yWindow="500" windowWidth="27640" windowHeight="26500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EPCI" sheetId="1" r:id="rId1"/>
-    <sheet name="Composition_communale" sheetId="2" r:id="rId2"/>
+    <sheet name="EPCI" sheetId="4" r:id="rId1"/>
+    <sheet name="Composition_communale" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Intercommunalité et Métropole</t>
   </si>
@@ -29,12 +29,6 @@
     <t>France - Liste des intercommunalités</t>
   </si>
   <si>
-    <t>Mise en ligne le 19/03/2021       Géographie au 01/01/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">©Insee       Source(s) : Insee, Code officiel géographique </t>
-  </si>
-  <si>
     <t>EPCI - Métropole</t>
   </si>
   <si>
@@ -132,44 +126,79 @@
   </si>
   <si>
     <t>28</t>
+  </si>
+  <si>
+    <t>200046977</t>
+  </si>
+  <si>
+    <t>Métropole de Lyon</t>
+  </si>
+  <si>
+    <t>METLYON</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>Mise en ligne le 17/03/2023       Géographie au 01/01/2023</t>
+  </si>
+  <si>
+    <t>@Insee       Source(s) : Insee, Code officiel géographique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF881423"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1E3269"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1E3269"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,63 +207,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
+        <fgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
+        <fgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -247,108 +231,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1535,310 +1437,255 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6266C9-A6CB-6242-AFEA-0F8AC9E745A2}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="55" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.1640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="13" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="16" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
+      <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="D7" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="7">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="21">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="22">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="22">
+      <c r="D10" s="7">
         <v>4</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A030296A-1333-A34D-9CD0-117CA01B62E5}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10" style="6" customWidth="1"/>
-    <col min="4" max="4" width="55" style="6" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="6" customWidth="1"/>
-    <col min="6" max="7" width="9.1640625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="6"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="58" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="E5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="F5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="13" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="F6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="16" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="19" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="D8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="11.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="E8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="F8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>